<commit_message>
recalculated output for the test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/calculation_output_4_specific_dates.xlsx
+++ b/src/main/resources/calculation_output_4_specific_dates.xlsx
@@ -379,13 +379,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9" style="1"/>
     <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -415,7 +416,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>17650</v>
+        <v>15150</v>
       </c>
       <c r="C3">
         <v>241</v>
@@ -426,10 +427,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>37915</v>
+        <v>37215</v>
       </c>
       <c r="C4">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -437,7 +438,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>86557</v>
+        <v>86700</v>
       </c>
       <c r="C5">
         <v>120</v>
@@ -448,7 +449,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>76177</v>
+        <v>76226</v>
       </c>
       <c r="C6">
         <v>135</v>

</xml_diff>